<commit_message>
delete duplicate spreadsheet and update results
</commit_message>
<xml_diff>
--- a/bott index quasicrystal.xlsx
+++ b/bott index quasicrystal.xlsx
@@ -5,12 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed quasicrystal" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="20x20" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="30x30" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="PBC 24x24" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="PBC 22x22" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="PBC 20x20" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="21">
   <si>
     <t xml:space="preserve">The two lines are fixed, and the system size is varied</t>
   </si>
@@ -66,7 +69,25 @@
     <t xml:space="preserve">system size</t>
   </si>
   <si>
+    <t xml:space="preserve">number of sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in quasicrystal</t>
+  </si>
+  <si>
     <t xml:space="preserve">oscillations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24x24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22x22</t>
   </si>
 </sst>
 </file>
@@ -181,7 +202,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -429,10 +450,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,6 +469,12 @@
         <v>8</v>
       </c>
       <c r="D1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -463,6 +490,9 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,7 +758,7 @@
         <v>-1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,6 +775,13 @@
       </c>
       <c r="I21" s="1" t="n">
         <v>-1</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <f aca="false">(K21/400)*100</f>
+        <v>85.75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,4 +1768,1487 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="G7" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>548</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <f aca="false">ROUND((K7/576)*100,2)</f>
+        <v>95.14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2" t="n">
+        <v>-9</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="G8" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>533</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <f aca="false">ROUND((K8/576)*100,2)</f>
+        <v>92.53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>515</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <f aca="false">ROUND((K9/576)*100,2)</f>
+        <v>89.41</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="G10" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>493</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <f aca="false">ROUND((K10/576)*100,2)</f>
+        <v>85.59</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="G11" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <f aca="false">ROUND((K11/576)*100,2)</f>
+        <v>81.42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="D12" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>441</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <f aca="false">ROUND((K12/576)*100,2)</f>
+        <v>76.56</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>410</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <f aca="false">ROUND((K13/576)*100,2)</f>
+        <v>71.18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="D15" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="G15" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>454</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <f aca="false">ROUND((K15/576)*100,2)</f>
+        <v>78.82</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="D16" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="G16" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>437</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <f aca="false">ROUND((K16/576)*100,2)</f>
+        <v>75.87</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="D17" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="G17" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>424</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <f aca="false">ROUND((K17/576)*100,2)</f>
+        <v>73.61</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="D19" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="G19" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <f aca="false">ROUND((K19/576)*100,2)</f>
+        <v>79.17</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="D20" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="G20" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>442</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <f aca="false">ROUND((K20/576)*100,2)</f>
+        <v>76.74</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="D21" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="G21" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>426</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <f aca="false">ROUND((K21/576)*100,2)</f>
+        <v>73.96</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="D22" s="2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="G22" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <f aca="false">ROUND((K22/576)*100,2)</f>
+        <v>70.83</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="D24" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="G24" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <f aca="false">ROUND((K24/576)*100,2)</f>
+        <v>74.13</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="D25" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="G25" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>411</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <f aca="false">ROUND((K25/576)*100,2)</f>
+        <v>71.35</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="D27" s="2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="G27" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <f aca="false">ROUND((K27/576)*100,2)</f>
+        <v>61.98</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="60">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="G7" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>451</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <f aca="false">ROUND((K7/484)*100,2)</f>
+        <v>93.18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="G8" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>434</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <f aca="false">ROUND((K8/484)*100,2)</f>
+        <v>89.67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>415</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <f aca="false">ROUND((K9/484)*100,2)</f>
+        <v>85.74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="G10" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>392</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <f aca="false">ROUND((K10/484)*100,2)</f>
+        <v>80.99</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="G11" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <f aca="false">ROUND((K11/484)*100,2)</f>
+        <v>75.83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="D12" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <f aca="false">ROUND((K12/484)*100,2)</f>
+        <v>69.83</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" s="2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <f aca="false">ROUND((K13/484)*100,2)</f>
+        <v>63.02</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="D14" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="G14" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <f aca="false">ROUND((K14/484)*100,2)</f>
+        <v>55.79</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="D16" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="G16" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <f aca="false">ROUND((K16/484)*100,2)</f>
+        <v>78.51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="D17" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="G17" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <f aca="false">ROUND((K17/484)*100,2)</f>
+        <v>75.62</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="D18" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="G18" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <f aca="false">ROUND((K18/484)*100,2)</f>
+        <v>72.93</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="58">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="1" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="G7" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <f aca="false">(K7/400)*100</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="G8" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <f aca="false">(K8/400)*100</f>
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <f aca="false">(K9/400)*100</f>
+        <v>90.25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="G10" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <f aca="false">(K10/400)*100</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="G11" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <f aca="false">(K11/400)*100</f>
+        <v>85.75</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="D12" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <f aca="false">(K12/400)*100</f>
+        <v>80.75</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" s="2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <f aca="false">(K13/400)*100</f>
+        <v>83.25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="D14" s="2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="G14" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <f aca="false">(K14/400)*100</f>
+        <v>83.25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="D15" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="G15" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <f aca="false">(K15/400)*100</f>
+        <v>80.25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="D16" s="2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="G16" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <f aca="false">(K16/400)*100</f>
+        <v>76.75</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="D17" s="2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="G17" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <f aca="false">(K17/400)*100</f>
+        <v>74.25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="D18" s="2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="G18" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <f aca="false">(K18/400)*100</f>
+        <v>71.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>